<commit_message>
Update 1 Des 2025
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11122"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbookpro/Desktop/Pengabdian Pasca/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A210E2-DF32-FB4D-B171-183F7DF1E781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676B897A-A7C8-2C4D-92D0-B9ABFED80197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15360" yWindow="1600" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10820" yWindow="1600" windowWidth="19420" windowHeight="11020" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KodePenyakit" sheetId="3" r:id="rId1"/>
     <sheet name="GejalaPenyakit" sheetId="4" r:id="rId2"/>
     <sheet name="Recording" sheetId="5" r:id="rId3"/>
+    <sheet name="Kepemilikan" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="155">
   <si>
     <t>Kode Gejala</t>
   </si>
@@ -423,6 +424,81 @@
   </si>
   <si>
     <t>Baru</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Nama</t>
+  </si>
+  <si>
+    <t>Kepemilikan Sapi</t>
+  </si>
+  <si>
+    <t>Jumlah yang berhasil di data</t>
+  </si>
+  <si>
+    <t>Induk</t>
+  </si>
+  <si>
+    <t>Bakalan induk</t>
+  </si>
+  <si>
+    <t>Bakalan Pejantan</t>
+  </si>
+  <si>
+    <t>Marsono Sopan</t>
+  </si>
+  <si>
+    <t>Sugino</t>
+  </si>
+  <si>
+    <t>Mad Sukardi</t>
+  </si>
+  <si>
+    <t>Slamet</t>
+  </si>
+  <si>
+    <t>A. Riyanto</t>
+  </si>
+  <si>
+    <t>Tukiman</t>
+  </si>
+  <si>
+    <t>Suwito</t>
+  </si>
+  <si>
+    <t>Didi Purnomo</t>
+  </si>
+  <si>
+    <t>Saiun</t>
+  </si>
+  <si>
+    <t>Sumiati</t>
+  </si>
+  <si>
+    <t>Karsimin</t>
+  </si>
+  <si>
+    <t>Erni Widyastuti</t>
+  </si>
+  <si>
+    <t>Sutarno</t>
+  </si>
+  <si>
+    <t>Tumilan</t>
+  </si>
+  <si>
+    <t>Sudarmin</t>
+  </si>
+  <si>
+    <t>Sujatmi</t>
+  </si>
+  <si>
+    <t>Sukadi</t>
+  </si>
+  <si>
+    <t>Udin</t>
   </si>
 </sst>
 </file>
@@ -446,7 +522,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -477,8 +553,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -538,11 +620,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -574,6 +682,25 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1394,7 +1521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{505BE5BE-6A57-914A-B52B-81ABE4E2630B}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:L6"/>
     </sheetView>
   </sheetViews>
@@ -1602,4 +1729,548 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50AC6233-4513-7E46-8F9D-3A040106A826}">
+  <dimension ref="A1:I21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:I21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="I2" s="14"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3" s="2">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2">
+        <v>4</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2">
+        <f>SUM(D3:H3)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2">
+        <f t="shared" ref="I4:I20" si="0">SUM(D4:H4)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C5" s="2">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2">
+        <v>2</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2">
+        <v>2</v>
+      </c>
+      <c r="I5" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C6" s="2">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2">
+        <v>7</v>
+      </c>
+      <c r="E6" s="2">
+        <v>3</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2">
+        <v>3</v>
+      </c>
+      <c r="I6" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C7" s="2">
+        <v>7</v>
+      </c>
+      <c r="D7" s="2">
+        <v>3</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" s="2">
+        <v>10</v>
+      </c>
+      <c r="D8" s="2">
+        <v>5</v>
+      </c>
+      <c r="E8" s="2">
+        <v>2</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2">
+        <v>2</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C9" s="2">
+        <v>23</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C10" s="2">
+        <v>6</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>2</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2">
+        <v>1</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C11" s="2">
+        <v>10</v>
+      </c>
+      <c r="D11" s="2">
+        <v>4</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2">
+        <v>2</v>
+      </c>
+      <c r="H11" s="2">
+        <v>4</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C12" s="2">
+        <v>8</v>
+      </c>
+      <c r="D12" s="2">
+        <v>2</v>
+      </c>
+      <c r="E12" s="2">
+        <v>4</v>
+      </c>
+      <c r="F12" s="2">
+        <v>2</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C13" s="2">
+        <v>6</v>
+      </c>
+      <c r="D13" s="2">
+        <v>3</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2">
+        <v>3</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C14" s="2">
+        <v>5</v>
+      </c>
+      <c r="D14" s="2">
+        <v>2</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2">
+        <v>2</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C15" s="2">
+        <v>3</v>
+      </c>
+      <c r="D15" s="2">
+        <v>2</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2">
+        <v>1</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C16" s="2">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2">
+        <v>1</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C17" s="2">
+        <v>6</v>
+      </c>
+      <c r="D17" s="2">
+        <v>2</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2">
+        <v>1</v>
+      </c>
+      <c r="H17" s="2">
+        <v>3</v>
+      </c>
+      <c r="I17" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C18" s="2">
+        <v>10</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C19" s="2">
+        <v>17</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C20" s="2">
+        <v>3</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1</v>
+      </c>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2">
+        <v>1</v>
+      </c>
+      <c r="I20" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="B21" s="19"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="2">
+        <f>SUM(D3:D20)</f>
+        <v>38</v>
+      </c>
+      <c r="E21" s="2">
+        <f t="shared" ref="E21:I21" si="1">SUM(E3:E20)</f>
+        <v>15</v>
+      </c>
+      <c r="F21" s="2">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="H21" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="I21" s="2">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="A21:B21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>